<commit_message>
moving files, cleaning indiv no file
</commit_message>
<xml_diff>
--- a/pheno_data/Photoguide_progress.xlsx
+++ b/pheno_data/Photoguide_progress.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deirdreloughnan/Documents/github/pheno_bc/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deirdreloughnan/Documents/github/pheno_bc/pheno_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0486E17-122C-8440-89DE-27A8240265B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AF40AE-4EC8-744A-BD87-611534E61FA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7600" yWindow="880" windowWidth="21940" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19840" yWindow="940" windowWidth="12740" windowHeight="20660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GC_splist" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="27">
   <si>
     <t>sp.name</t>
   </si>
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,6 +1033,9 @@
       <c r="G2" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1056,6 +1059,9 @@
       <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1068,9 +1074,21 @@
       <c r="D4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1114,6 +1132,12 @@
         <v>25</v>
       </c>
       <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1135,6 +1159,9 @@
       <c r="G7" t="s">
         <v>25</v>
       </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1155,7 +1182,12 @@
       <c r="F8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="I8" t="s">
         <v>25</v>
       </c>
@@ -1177,7 +1209,9 @@
         <v>25</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1195,7 +1229,9 @@
       <c r="F10" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1216,6 +1252,12 @@
       <c r="G11" t="s">
         <v>25</v>
       </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1231,6 +1273,9 @@
         <v>25</v>
       </c>
       <c r="F12" s="1"/>
+      <c r="G12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1257,6 +1302,9 @@
       <c r="H13" t="s">
         <v>25</v>
       </c>
+      <c r="I13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1280,6 +1328,9 @@
       <c r="G14" t="s">
         <v>25</v>
       </c>
+      <c r="H14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1300,6 +1351,9 @@
       <c r="G15" t="s">
         <v>25</v>
       </c>
+      <c r="H15" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1320,7 +1374,12 @@
       <c r="F16" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -1361,6 +1420,9 @@
       <c r="F18" t="s">
         <v>25</v>
       </c>
+      <c r="H18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -1424,6 +1486,9 @@
       <c r="G21" t="s">
         <v>25</v>
       </c>
+      <c r="H21" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -1439,6 +1504,9 @@
         <v>25</v>
       </c>
       <c r="F22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
moved files, cleaned indiv no
</commit_message>
<xml_diff>
--- a/pheno_data/Photoguide_progress.xlsx
+++ b/pheno_data/Photoguide_progress.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deirdreloughnan/Documents/github/pheno_bc/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deirdreloughnan/Documents/github/pheno_bc/pheno_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0486E17-122C-8440-89DE-27A8240265B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AF40AE-4EC8-744A-BD87-611534E61FA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7600" yWindow="880" windowWidth="21940" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19840" yWindow="940" windowWidth="12740" windowHeight="20660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GC_splist" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="27">
   <si>
     <t>sp.name</t>
   </si>
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,6 +1033,9 @@
       <c r="G2" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1056,6 +1059,9 @@
       <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1068,9 +1074,21 @@
       <c r="D4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1114,6 +1132,12 @@
         <v>25</v>
       </c>
       <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1135,6 +1159,9 @@
       <c r="G7" t="s">
         <v>25</v>
       </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1155,7 +1182,12 @@
       <c r="F8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="I8" t="s">
         <v>25</v>
       </c>
@@ -1177,7 +1209,9 @@
         <v>25</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1195,7 +1229,9 @@
       <c r="F10" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1216,6 +1252,12 @@
       <c r="G11" t="s">
         <v>25</v>
       </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1231,6 +1273,9 @@
         <v>25</v>
       </c>
       <c r="F12" s="1"/>
+      <c r="G12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1257,6 +1302,9 @@
       <c r="H13" t="s">
         <v>25</v>
       </c>
+      <c r="I13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1280,6 +1328,9 @@
       <c r="G14" t="s">
         <v>25</v>
       </c>
+      <c r="H14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1300,6 +1351,9 @@
       <c r="G15" t="s">
         <v>25</v>
       </c>
+      <c r="H15" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1320,7 +1374,12 @@
       <c r="F16" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -1361,6 +1420,9 @@
       <c r="F18" t="s">
         <v>25</v>
       </c>
+      <c r="H18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -1424,6 +1486,9 @@
       <c r="G21" t="s">
         <v>25</v>
       </c>
+      <c r="H21" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -1439,6 +1504,9 @@
         <v>25</v>
       </c>
       <c r="F22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>